<commit_message>
num of quiz inputable.
</commit_message>
<xml_diff>
--- a/resources/quiz/quizjs.xlsx
+++ b/resources/quiz/quizjs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\POMK\Src\Medicalpark2024\resources\quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD7BBF7-ACCC-45AE-92DF-27317C67CA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1730C676-56EC-41D4-A91A-EB8E2F797085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="画像ファイル変換" sheetId="2" r:id="rId1"/>
     <sheet name="質問リスト" sheetId="1" r:id="rId2"/>
+    <sheet name="設定" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="52">
   <si>
     <t>質問</t>
   </si>
@@ -253,7 +254,30 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>slpeen.png</t>
+    <t>spleen.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>問題数</t>
+    <rPh sb="0" eb="2">
+      <t>モンダイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>スウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一問あたりの解答時間</t>
+    <rPh sb="0" eb="2">
+      <t>イチモン</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カイトウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ジカン</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -284,7 +308,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,6 +474,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -726,9 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5463B239-CAF8-46A9-A718-7B2DB4A4D1B0}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -810,7 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -1472,7 +1502,7 @@
   IF(E32&lt;&gt;"",", ""images/" &amp; VLOOKUP(E32,画像ファイル変換!A:B,2,FALSE) &amp; """",""),
   IF(F32&lt;&gt;"",", ""images/" &amp; VLOOKUP(F32,画像ファイル変換!A:B,2,FALSE) &amp; """",""),
   IF(G32&lt;&gt;"",", ""images/" &amp; VLOOKUP(G32,画像ファイル変換!A:B,2,FALSE) &amp; """","")) &amp; "]")</f>
-        <v>["images/slpeen.png", "images/liver.png"]</v>
+        <v>["images/spleen.png", "images/liver.png"]</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>41</v>
@@ -1731,4 +1761,39 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5A4893-007B-4876-84E9-8A2500C2A902}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="15">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>